<commit_message>
Revert "Merge branch 'master' of https://github.com/fairwood/WarOfStarship"
This reverts commit bf92beb3d51ffacd0350b9bf186100f94a7d1478, reversing
changes made to 164cd0a4aa8fb27dfb4171d52bceecb831a44c3c.
</commit_message>
<xml_diff>
--- a/Client/assets/Csv/Building.xlsx
+++ b/Client/assets/Csv/Building.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\WarOfStarship\Client\assets\Csv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\WarOfStarship\Client\assets\Csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">工作表1!$A$1:$K$1</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -93,6 +93,22 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>战斗机生产车间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>战斗机机库</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>轰炸机生产车间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>轰炸机机库</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>激光炮生产车间</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -234,29 +250,13 @@
   </si>
   <si>
     <t>_upgradeRate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>攻击机机库</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>攻击机生产车间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>护卫机生产车间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>护卫机机库</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2">
     <font>
       <sz val="12"/>
@@ -579,10 +579,10 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -600,25 +600,25 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
       </c>
       <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" t="s">
-        <v>29</v>
-      </c>
       <c r="G1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="I1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="J1" t="s">
         <v>2</v>
@@ -627,16 +627,16 @@
         <v>3</v>
       </c>
       <c r="L1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="M1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="N1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="O1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -647,13 +647,13 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D2">
         <v>10</v>
       </c>
       <c r="J2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="K2">
         <v>10</v>
@@ -662,18 +662,18 @@
         <v>4</v>
       </c>
       <c r="O2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -685,7 +685,7 @@
         <v>3</v>
       </c>
       <c r="O3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -696,13 +696,13 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D4">
         <v>20</v>
       </c>
       <c r="J4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="K4">
         <v>5</v>
@@ -711,18 +711,18 @@
         <v>4</v>
       </c>
       <c r="O4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D5">
         <v>100</v>
@@ -734,7 +734,7 @@
         <v>3</v>
       </c>
       <c r="O5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -742,28 +742,28 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D6">
         <v>100</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G6">
         <v>30</v>
       </c>
       <c r="H6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="I6">
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="L6">
         <v>0.25</v>
@@ -780,10 +780,10 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D7">
         <v>50</v>
@@ -800,28 +800,28 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D8">
         <v>160</v>
       </c>
       <c r="F8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="G8">
         <v>50</v>
       </c>
       <c r="H8" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="I8">
         <v>2</v>
       </c>
       <c r="J8" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="L8">
         <v>0.33329999999999999</v>
@@ -838,10 +838,10 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D9">
         <v>80</v>
@@ -858,28 +858,28 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D10">
         <v>80</v>
       </c>
       <c r="F10" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="G10">
         <v>25</v>
       </c>
       <c r="H10" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L10">
         <v>0.2</v>
@@ -896,10 +896,10 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D11">
         <v>200</v>
@@ -916,28 +916,28 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D12">
         <v>2000</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="G12">
         <v>10000</v>
       </c>
       <c r="H12" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="I12">
         <v>10000</v>
       </c>
       <c r="J12" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="L12">
         <v>24</v>
@@ -954,10 +954,10 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D13">
         <v>1000</v>
@@ -971,10 +971,10 @@
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D14">
         <v>5</v>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'master' of https://github.com/fairwood/WarOfStarship""
This reverts commit a0c1b62bacaa626f33c4a2438a0fa129ae9959f0.
</commit_message>
<xml_diff>
--- a/Client/assets/Csv/Building.xlsx
+++ b/Client/assets/Csv/Building.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\WarOfStarship\Client\assets\Csv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\WarOfStarship\Client\assets\Csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">工作表1!$A$1:$K$1</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -93,22 +93,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>战斗机生产车间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>战斗机机库</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>轰炸机生产车间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>轰炸机机库</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>激光炮生产车间</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -250,13 +234,29 @@
   </si>
   <si>
     <t>_upgradeRate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击机机库</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击机生产车间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>护卫机生产车间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>护卫机机库</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2">
     <font>
       <sz val="12"/>
@@ -579,10 +579,10 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -600,25 +600,25 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J1" t="s">
         <v>2</v>
@@ -627,16 +627,16 @@
         <v>3</v>
       </c>
       <c r="L1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="M1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="N1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="O1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -647,13 +647,13 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D2">
         <v>10</v>
       </c>
       <c r="J2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="K2">
         <v>10</v>
@@ -662,18 +662,18 @@
         <v>4</v>
       </c>
       <c r="O2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -685,7 +685,7 @@
         <v>3</v>
       </c>
       <c r="O3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -696,13 +696,13 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D4">
         <v>20</v>
       </c>
       <c r="J4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="K4">
         <v>5</v>
@@ -711,18 +711,18 @@
         <v>4</v>
       </c>
       <c r="O4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D5">
         <v>100</v>
@@ -734,7 +734,7 @@
         <v>3</v>
       </c>
       <c r="O5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -742,28 +742,28 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D6">
         <v>100</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G6">
         <v>30</v>
       </c>
       <c r="H6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I6">
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="L6">
         <v>0.25</v>
@@ -780,10 +780,10 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D7">
         <v>50</v>
@@ -800,28 +800,28 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D8">
         <v>160</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G8">
         <v>50</v>
       </c>
       <c r="H8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I8">
         <v>2</v>
       </c>
       <c r="J8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L8">
         <v>0.33329999999999999</v>
@@ -838,10 +838,10 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D9">
         <v>80</v>
@@ -858,28 +858,28 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D10">
         <v>80</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G10">
         <v>25</v>
       </c>
       <c r="H10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="L10">
         <v>0.2</v>
@@ -896,10 +896,10 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D11">
         <v>200</v>
@@ -916,28 +916,28 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
         <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
       </c>
       <c r="D12">
         <v>2000</v>
       </c>
       <c r="F12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G12">
         <v>10000</v>
       </c>
       <c r="H12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I12">
         <v>10000</v>
       </c>
       <c r="J12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L12">
         <v>24</v>
@@ -954,10 +954,10 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
         <v>24</v>
-      </c>
-      <c r="C13" t="s">
-        <v>28</v>
       </c>
       <c r="D13">
         <v>1000</v>
@@ -971,10 +971,10 @@
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D14">
         <v>5</v>

</xml_diff>